<commit_message>
reworked first draft for midwest macro submission
I think it's a whole lot better
</commit_message>
<xml_diff>
--- a/literature/record_opt_monpol_learning.xlsx
+++ b/literature/record_opt_monpol_learning.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3340" yWindow="600" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Paper / book</t>
   </si>
@@ -61,6 +61,33 @@
   </si>
   <si>
     <t>Gaspar et al 2011</t>
+  </si>
+  <si>
+    <t>Molnar Santoro 2014</t>
+  </si>
+  <si>
+    <t>optimal monpol under adaptive EE learning involves a new intertemporal tradeoff in which CB foregoes short-run stabilization in order to facilitate learning</t>
+  </si>
+  <si>
+    <t>Gaspar et al 2006</t>
+  </si>
+  <si>
+    <t>CB reacts more persistently to cost-push shocks</t>
+  </si>
+  <si>
+    <t>Hbook chapter</t>
+  </si>
+  <si>
+    <t>Ferrero 2007</t>
+  </si>
+  <si>
+    <t>more aggressive monpol increases the speed of convergence, but high speed is not always desirable</t>
+  </si>
+  <si>
+    <t>Eusepi et al, 2018, Limits</t>
+  </si>
+  <si>
+    <t>due to the gain, monetary policy faces limits</t>
   </si>
 </sst>
 </file>
@@ -479,16 +506,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="35.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="105.1640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="134.6640625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1">
@@ -548,7 +575,42 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
         <v>13</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
some thinking about particular solutions of nonautonomous difference equations
</commit_message>
<xml_diff>
--- a/literature/record_opt_monpol_learning.xlsx
+++ b/literature/record_opt_monpol_learning.xlsx
@@ -75,9 +75,6 @@
     <t>CB reacts more persistently to cost-push shocks</t>
   </si>
   <si>
-    <t>Hbook chapter</t>
-  </si>
-  <si>
     <t>Ferrero 2007</t>
   </si>
   <si>
@@ -88,6 +85,9 @@
   </si>
   <si>
     <t>due to the gain, monetary policy faces limits</t>
+  </si>
+  <si>
+    <t>Hbook chapter - adaptive learning (dgain and cgain) is ultimately the same as RE but learning introduces an intertemporal tradeoff that wasn't there before</t>
   </si>
 </sst>
 </file>
@@ -509,7 +509,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -586,7 +586,7 @@
         <v>13</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -599,18 +599,18 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added lit, typed up materials21 some
</commit_message>
<xml_diff>
--- a/literature/record_opt_monpol_learning.xlsx
+++ b/literature/record_opt_monpol_learning.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Paper / book</t>
   </si>
@@ -88,6 +88,18 @@
   </si>
   <si>
     <t>Hbook chapter - adaptive learning (dgain and cgain) is ultimately the same as RE but learning introduces an intertemporal tradeoff that wasn't there before</t>
+  </si>
+  <si>
+    <t>Hommes, JEL,2019/20</t>
+  </si>
+  <si>
+    <t>mon pol should be more aggressive on things to add negative feedback, makes the system more stable</t>
+  </si>
+  <si>
+    <t>Gabaix 2019, bounded rational NK</t>
+  </si>
+  <si>
+    <t>opt mon pol isn't price level targeting - truly, the more BR firms are, the less forward-looking, and the less commitment the CB can implement.</t>
   </si>
 </sst>
 </file>
@@ -506,10 +518,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -613,6 +625,22 @@
         <v>21</v>
       </c>
     </row>
+    <row r="12" spans="1:7">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
added SPF one-year ahead
</commit_message>
<xml_diff>
--- a/literature/record_opt_monpol_learning.xlsx
+++ b/literature/record_opt_monpol_learning.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Paper / book</t>
   </si>
@@ -100,18 +100,25 @@
   </si>
   <si>
     <t>opt mon pol isn't price level targeting - truly, the more BR firms are, the less forward-looking, and the less commitment the CB can implement.</t>
+  </si>
+  <si>
+    <t>Gobbi et al, 2019</t>
+  </si>
+  <si>
+    <t>the prob which agents assign to switching to liquidity trap regime is a metric for deanchoring. This prob, p, is determined via a logistic equation of the output gap. The model reconciles the empirical observations that 1) missing deflation + inflation, 2) de-anchoring of expectations and 3) steepening Phillips Curve (in terms of pi and x, in terms of pi and u, flattening). It also suggests that a Taylor rule may not be enough, even if aggressive, if shocks are big enough.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -136,6 +143,13 @@
       <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -171,7 +185,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -179,6 +193,10 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -518,10 +536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -625,11 +643,11 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
-      <c r="A12" t="s">
+    <row r="12" spans="1:7" s="5" customFormat="1">
+      <c r="A12" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="6" t="s">
         <v>24</v>
       </c>
     </row>
@@ -639,6 +657,14 @@
       </c>
       <c r="B13" s="2" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="45">
+      <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
more work on prezi
</commit_message>
<xml_diff>
--- a/literature/record_opt_monpol_learning.xlsx
+++ b/literature/record_opt_monpol_learning.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="2100" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="67960" yWindow="-2180" windowWidth="25600" windowHeight="15600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Paper / book</t>
   </si>
@@ -106,6 +106,12 @@
   </si>
   <si>
     <t>the prob which agents assign to switching to liquidity trap regime is a metric for deanchoring. This prob, p, is determined via a logistic equation of the output gap. The model reconciles the empirical observations that 1) missing deflation + inflation, 2) de-anchoring of expectations and 3) steepening Phillips Curve (in terms of pi and x, in terms of pi and u, flattening). It also suggests that a Taylor rule may not be enough, even if aggressive, if shocks are big enough.</t>
+  </si>
+  <si>
+    <t>Mele et al 2019</t>
+  </si>
+  <si>
+    <t>optimal monpol under dgain learning isnt PLT, its inflation targeting</t>
   </si>
 </sst>
 </file>
@@ -535,10 +541,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -666,6 +672,14 @@
         <v>28</v>
       </c>
     </row>
+    <row r="15" spans="1:7">
+      <c r="A15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>